<commit_message>
Added field descriptions for BLS data
</commit_message>
<xml_diff>
--- a/Excel files to merge/indeed draft output.xlsx
+++ b/Excel files to merge/indeed draft output.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjrhi\OneDrive\Documents\GitHub\Course-Job-Match\Excel files to merge\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_F1225CDC97D9AEFF0BF392360E1C3B5A45674598" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{0ED9F897-0383-4082-81BF-3301C6133E54}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="910" yWindow="1070" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -667,8 +673,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -744,6 +750,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -790,7 +804,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -822,9 +836,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -856,6 +888,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1031,14 +1081,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="255.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1061,7 +1118,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1087,7 +1144,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1113,7 +1170,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1139,7 +1196,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1165,7 +1222,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1191,7 +1248,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1217,7 +1274,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1243,7 +1300,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1269,7 +1326,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1295,7 +1352,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1321,7 +1378,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1347,7 +1404,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1373,7 +1430,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1399,7 +1456,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1427,20 +1484,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F8" r:id="rId7"/>
-    <hyperlink ref="F9" r:id="rId8"/>
-    <hyperlink ref="F10" r:id="rId9"/>
-    <hyperlink ref="F11" r:id="rId10"/>
-    <hyperlink ref="F12" r:id="rId11"/>
-    <hyperlink ref="F13" r:id="rId12"/>
-    <hyperlink ref="F14" r:id="rId13"/>
-    <hyperlink ref="F15" r:id="rId14"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>